<commit_message>
New version with tune function
</commit_message>
<xml_diff>
--- a/pitches.xlsx
+++ b/pitches.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbertello/Programmes/accordage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E85BCC1-D52A-8643-8DA3-4790B6EC540A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B7C6BB-7268-DE4F-A9E7-344C787C3D65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="20400" windowHeight="15400" xr2:uid="{3B3C9344-3A85-CC43-AC78-C1B0E7E14E68}"/>
+    <workbookView xWindow="3720" yWindow="460" windowWidth="20400" windowHeight="15400" xr2:uid="{3B3C9344-3A85-CC43-AC78-C1B0E7E14E68}"/>
   </bookViews>
   <sheets>
-    <sheet name="Harmonique" sheetId="1" r:id="rId1"/>
-    <sheet name="3ce" sheetId="2" r:id="rId2"/>
-    <sheet name="4te" sheetId="3" r:id="rId3"/>
-    <sheet name="5te" sheetId="4" r:id="rId4"/>
-    <sheet name="6te" sheetId="5" r:id="rId5"/>
+    <sheet name="Intervalles" sheetId="6" r:id="rId1"/>
+    <sheet name="Harmoniques" sheetId="1" r:id="rId2"/>
+    <sheet name="3ce" sheetId="2" r:id="rId3"/>
+    <sheet name="4te" sheetId="3" r:id="rId4"/>
+    <sheet name="5te" sheetId="4" r:id="rId5"/>
+    <sheet name="6te" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="89">
   <si>
     <t>FA3</t>
   </si>
@@ -301,6 +302,9 @@
   </si>
   <si>
     <t>DO8</t>
+  </si>
+  <si>
+    <t>SOL3</t>
   </si>
 </sst>
 </file>
@@ -323,12 +327,66 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -343,10 +401,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -660,10 +728,1438 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C73B3670-ECCA-1245-9765-CA1D69B4CF6C}">
+  <dimension ref="A1:J41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C2" s="2">
+        <v>440</v>
+      </c>
+      <c r="D2" s="2">
+        <f>$C2*D$1</f>
+        <v>880</v>
+      </c>
+      <c r="E2" s="2">
+        <f>$C2*E$1</f>
+        <v>1320</v>
+      </c>
+      <c r="F2" s="2">
+        <f>$C2*F$1</f>
+        <v>1760</v>
+      </c>
+      <c r="G2" s="2">
+        <f>$C2*G$1</f>
+        <v>2200</v>
+      </c>
+      <c r="H2" s="2">
+        <f>$C2*H$1</f>
+        <v>2640</v>
+      </c>
+      <c r="I2" s="2">
+        <f>$C2*I$1</f>
+        <v>3080</v>
+      </c>
+      <c r="J2" s="2">
+        <f>$C2*J$1</f>
+        <v>3520</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="3">
+        <v>-19</v>
+      </c>
+      <c r="C4" s="2">
+        <f>C$2*2^($B4/12)</f>
+        <v>146.83238395870382</v>
+      </c>
+      <c r="D4" s="2">
+        <f>$C4*D$1</f>
+        <v>293.66476791740763</v>
+      </c>
+      <c r="E4" s="2">
+        <f>$C4*E$1</f>
+        <v>440.49715187611145</v>
+      </c>
+      <c r="F4" s="2">
+        <f>$C4*F$1</f>
+        <v>587.32953583481526</v>
+      </c>
+      <c r="G4" s="2">
+        <f>$C4*G$1</f>
+        <v>734.16191979351902</v>
+      </c>
+      <c r="H4" s="2">
+        <f>$C4*H$1</f>
+        <v>880.99430375222289</v>
+      </c>
+      <c r="I4" s="2">
+        <f>$C4*I$1</f>
+        <v>1027.8266877109268</v>
+      </c>
+      <c r="J4" s="2">
+        <f>$C4*J$1</f>
+        <v>1174.6590716696305</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <v>-18</v>
+      </c>
+      <c r="C5" s="2">
+        <f>C$2*2^($B5/12)</f>
+        <v>155.56349186104046</v>
+      </c>
+      <c r="D5" s="2">
+        <f>$C5*D$1</f>
+        <v>311.12698372208092</v>
+      </c>
+      <c r="E5" s="2">
+        <f>$C5*E$1</f>
+        <v>466.69047558312138</v>
+      </c>
+      <c r="F5" s="2">
+        <f>$C5*F$1</f>
+        <v>622.25396744416184</v>
+      </c>
+      <c r="G5" s="2">
+        <f>$C5*G$1</f>
+        <v>777.81745930520231</v>
+      </c>
+      <c r="H5" s="2">
+        <f>$C5*H$1</f>
+        <v>933.38095116624277</v>
+      </c>
+      <c r="I5" s="2">
+        <f>$C5*I$1</f>
+        <v>1088.9444430272833</v>
+      </c>
+      <c r="J5" s="2">
+        <f>$C5*J$1</f>
+        <v>1244.5079348883237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="3">
+        <v>-17</v>
+      </c>
+      <c r="C6" s="2">
+        <f>C$2*2^($B6/12)</f>
+        <v>164.81377845643496</v>
+      </c>
+      <c r="D6" s="2">
+        <f>$C6*D$1</f>
+        <v>329.62755691286992</v>
+      </c>
+      <c r="E6" s="2">
+        <f>$C6*E$1</f>
+        <v>494.44133536930485</v>
+      </c>
+      <c r="F6" s="2">
+        <f>$C6*F$1</f>
+        <v>659.25511382573984</v>
+      </c>
+      <c r="G6" s="2">
+        <f>$C6*G$1</f>
+        <v>824.06889228217483</v>
+      </c>
+      <c r="H6" s="2">
+        <f>$C6*H$1</f>
+        <v>988.8826707386097</v>
+      </c>
+      <c r="I6" s="2">
+        <f>$C6*I$1</f>
+        <v>1153.6964491950448</v>
+      </c>
+      <c r="J6" s="2">
+        <f>$C6*J$1</f>
+        <v>1318.5102276514797</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>-16</v>
+      </c>
+      <c r="C7" s="2">
+        <f>C$2*2^($B7/12)</f>
+        <v>174.61411571650197</v>
+      </c>
+      <c r="D7" s="2">
+        <f>$C7*D$1</f>
+        <v>349.22823143300394</v>
+      </c>
+      <c r="E7" s="2">
+        <f>$C7*E$1</f>
+        <v>523.84234714950594</v>
+      </c>
+      <c r="F7" s="2">
+        <f>$C7*F$1</f>
+        <v>698.45646286600788</v>
+      </c>
+      <c r="G7" s="2">
+        <f>$C7*G$1</f>
+        <v>873.07057858250982</v>
+      </c>
+      <c r="H7" s="2">
+        <f>$C7*H$1</f>
+        <v>1047.6846942990119</v>
+      </c>
+      <c r="I7" s="2">
+        <f>$C7*I$1</f>
+        <v>1222.2988100155137</v>
+      </c>
+      <c r="J7" s="2">
+        <f>$C7*J$1</f>
+        <v>1396.9129257320158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>-15</v>
+      </c>
+      <c r="C8" s="2">
+        <f>C$2*2^($B8/12)</f>
+        <v>184.99721135581723</v>
+      </c>
+      <c r="D8" s="2">
+        <f>$C8*D$1</f>
+        <v>369.99442271163446</v>
+      </c>
+      <c r="E8" s="2">
+        <f>$C8*E$1</f>
+        <v>554.99163406745174</v>
+      </c>
+      <c r="F8" s="2">
+        <f>$C8*F$1</f>
+        <v>739.98884542326891</v>
+      </c>
+      <c r="G8" s="2">
+        <f>$C8*G$1</f>
+        <v>924.98605677908608</v>
+      </c>
+      <c r="H8" s="2">
+        <f>$C8*H$1</f>
+        <v>1109.9832681349035</v>
+      </c>
+      <c r="I8" s="2">
+        <f>$C8*I$1</f>
+        <v>1294.9804794907207</v>
+      </c>
+      <c r="J8" s="2">
+        <f>$C8*J$1</f>
+        <v>1479.9776908465378</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="3">
+        <v>-14</v>
+      </c>
+      <c r="C9" s="2">
+        <f>C$2*2^($B9/12)</f>
+        <v>195.99771799087463</v>
+      </c>
+      <c r="D9" s="2">
+        <f>$C9*D$1</f>
+        <v>391.99543598174927</v>
+      </c>
+      <c r="E9" s="2">
+        <f>$C9*E$1</f>
+        <v>587.99315397262387</v>
+      </c>
+      <c r="F9" s="2">
+        <f>$C9*F$1</f>
+        <v>783.99087196349853</v>
+      </c>
+      <c r="G9" s="2">
+        <f>$C9*G$1</f>
+        <v>979.9885899543732</v>
+      </c>
+      <c r="H9" s="2">
+        <f>$C9*H$1</f>
+        <v>1175.9863079452477</v>
+      </c>
+      <c r="I9" s="2">
+        <f>$C9*I$1</f>
+        <v>1371.9840259361224</v>
+      </c>
+      <c r="J9" s="2">
+        <f>$C9*J$1</f>
+        <v>1567.9817439269971</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>-13</v>
+      </c>
+      <c r="C10" s="2">
+        <f>C$2*2^($B10/12)</f>
+        <v>207.65234878997259</v>
+      </c>
+      <c r="D10" s="2">
+        <f>$C10*D$1</f>
+        <v>415.30469757994518</v>
+      </c>
+      <c r="E10" s="2">
+        <f>$C10*E$1</f>
+        <v>622.95704636991775</v>
+      </c>
+      <c r="F10" s="2">
+        <f>$C10*F$1</f>
+        <v>830.60939515989037</v>
+      </c>
+      <c r="G10" s="2">
+        <f>$C10*G$1</f>
+        <v>1038.2617439498629</v>
+      </c>
+      <c r="H10" s="2">
+        <f>$C10*H$1</f>
+        <v>1245.9140927398355</v>
+      </c>
+      <c r="I10" s="2">
+        <f>$C10*I$1</f>
+        <v>1453.5664415298081</v>
+      </c>
+      <c r="J10" s="2">
+        <f>$C10*J$1</f>
+        <v>1661.2187903197807</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4">
+        <v>-12</v>
+      </c>
+      <c r="C11" s="4">
+        <f>C$2*2^($B11/12)</f>
+        <v>220</v>
+      </c>
+      <c r="D11" s="5">
+        <f>$C11*D$1</f>
+        <v>440</v>
+      </c>
+      <c r="E11" s="11">
+        <f>$C11*E$1</f>
+        <v>660</v>
+      </c>
+      <c r="F11" s="8">
+        <f>$C11*F$1</f>
+        <v>880</v>
+      </c>
+      <c r="G11" s="10">
+        <f>$C11*G$1</f>
+        <v>1100</v>
+      </c>
+      <c r="H11" s="7">
+        <f>$C11*H$1</f>
+        <v>1320</v>
+      </c>
+      <c r="I11" s="9">
+        <f>$C11*I$1</f>
+        <v>1540</v>
+      </c>
+      <c r="J11" s="6">
+        <f>$C11*J$1</f>
+        <v>1760</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>-11</v>
+      </c>
+      <c r="C12" s="2">
+        <f>C$2*2^($B12/12)</f>
+        <v>233.08188075904496</v>
+      </c>
+      <c r="D12" s="2">
+        <f>$C12*D$1</f>
+        <v>466.16376151808993</v>
+      </c>
+      <c r="E12" s="2">
+        <f>$C12*E$1</f>
+        <v>699.24564227713495</v>
+      </c>
+      <c r="F12" s="2">
+        <f>$C12*F$1</f>
+        <v>932.32752303617985</v>
+      </c>
+      <c r="G12" s="2">
+        <f>$C12*G$1</f>
+        <v>1165.4094037952248</v>
+      </c>
+      <c r="H12" s="2">
+        <f>$C12*H$1</f>
+        <v>1398.4912845542699</v>
+      </c>
+      <c r="I12" s="2">
+        <f>$C12*I$1</f>
+        <v>1631.5731653133148</v>
+      </c>
+      <c r="J12" s="2">
+        <f>$C12*J$1</f>
+        <v>1864.6550460723597</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="3">
+        <v>-10</v>
+      </c>
+      <c r="C13" s="2">
+        <f>C$2*2^($B13/12)</f>
+        <v>246.94165062806206</v>
+      </c>
+      <c r="D13" s="2">
+        <f>$C13*D$1</f>
+        <v>493.88330125612413</v>
+      </c>
+      <c r="E13" s="2">
+        <f>$C13*E$1</f>
+        <v>740.82495188418625</v>
+      </c>
+      <c r="F13" s="2">
+        <f>$C13*F$1</f>
+        <v>987.76660251224826</v>
+      </c>
+      <c r="G13" s="2">
+        <f>$C13*G$1</f>
+        <v>1234.7082531403103</v>
+      </c>
+      <c r="H13" s="12">
+        <f>$C13*H$1</f>
+        <v>1481.6499037683725</v>
+      </c>
+      <c r="I13" s="6">
+        <f>$C13*I$1</f>
+        <v>1728.5915543964345</v>
+      </c>
+      <c r="J13" s="2">
+        <f>$C13*J$1</f>
+        <v>1975.5332050244965</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>-9</v>
+      </c>
+      <c r="C14" s="2">
+        <f>C$2*2^($B14/12)</f>
+        <v>261.62556530059862</v>
+      </c>
+      <c r="D14" s="2">
+        <f>$C14*D$1</f>
+        <v>523.25113060119725</v>
+      </c>
+      <c r="E14" s="2">
+        <f>$C14*E$1</f>
+        <v>784.87669590179587</v>
+      </c>
+      <c r="F14" s="2">
+        <f>$C14*F$1</f>
+        <v>1046.5022612023945</v>
+      </c>
+      <c r="G14" s="7">
+        <f>$C14*G$1</f>
+        <v>1308.1278265029932</v>
+      </c>
+      <c r="H14" s="9">
+        <f>$C14*H$1</f>
+        <v>1569.7533918035917</v>
+      </c>
+      <c r="I14" s="2">
+        <f>$C14*I$1</f>
+        <v>1831.3789571041902</v>
+      </c>
+      <c r="J14" s="2">
+        <f>$C14*J$1</f>
+        <v>2093.004522404789</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>-8</v>
+      </c>
+      <c r="C15" s="2">
+        <f>C$2*2^($B15/12)</f>
+        <v>277.18263097687208</v>
+      </c>
+      <c r="D15" s="2">
+        <f>$C15*D$1</f>
+        <v>554.36526195374415</v>
+      </c>
+      <c r="E15" s="2">
+        <f>$C15*E$1</f>
+        <v>831.54789293061617</v>
+      </c>
+      <c r="F15" s="10">
+        <f>$C15*F$1</f>
+        <v>1108.7305239074883</v>
+      </c>
+      <c r="G15" s="2">
+        <f>$C15*G$1</f>
+        <v>1385.9131548843604</v>
+      </c>
+      <c r="H15" s="2">
+        <f>$C15*H$1</f>
+        <v>1663.0957858612323</v>
+      </c>
+      <c r="I15" s="2">
+        <f>$C15*I$1</f>
+        <v>1940.2784168381045</v>
+      </c>
+      <c r="J15" s="2">
+        <f>$C15*J$1</f>
+        <v>2217.4610478149766</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="3">
+        <v>-7</v>
+      </c>
+      <c r="C16" s="2">
+        <f>C$2*2^($B16/12)</f>
+        <v>293.66476791740757</v>
+      </c>
+      <c r="D16" s="2">
+        <f>$C16*D$1</f>
+        <v>587.32953583481515</v>
+      </c>
+      <c r="E16" s="8">
+        <f>$C16*E$1</f>
+        <v>880.99430375222278</v>
+      </c>
+      <c r="F16" s="2">
+        <f>$C16*F$1</f>
+        <v>1174.6590716696303</v>
+      </c>
+      <c r="G16" s="2">
+        <f>$C16*G$1</f>
+        <v>1468.3238395870378</v>
+      </c>
+      <c r="H16" s="6">
+        <f>$C16*H$1</f>
+        <v>1761.9886075044456</v>
+      </c>
+      <c r="I16" s="2">
+        <f>$C16*I$1</f>
+        <v>2055.6533754218531</v>
+      </c>
+      <c r="J16" s="2">
+        <f>$C16*J$1</f>
+        <v>2349.3181433392606</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <v>-6</v>
+      </c>
+      <c r="C17" s="2">
+        <f>C$2*2^($B17/12)</f>
+        <v>311.12698372208087</v>
+      </c>
+      <c r="D17" s="2">
+        <f>$C17*D$1</f>
+        <v>622.25396744416173</v>
+      </c>
+      <c r="E17" s="2">
+        <f>$C17*E$1</f>
+        <v>933.38095116624254</v>
+      </c>
+      <c r="F17" s="2">
+        <f>$C17*F$1</f>
+        <v>1244.5079348883235</v>
+      </c>
+      <c r="G17" s="9">
+        <f>$C17*G$1</f>
+        <v>1555.6349186104044</v>
+      </c>
+      <c r="H17" s="2">
+        <f>$C17*H$1</f>
+        <v>1866.7619023324851</v>
+      </c>
+      <c r="I17" s="2">
+        <f>$C17*I$1</f>
+        <v>2177.8888860545662</v>
+      </c>
+      <c r="J17" s="2">
+        <f>$C17*J$1</f>
+        <v>2489.0158697766469</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="3">
+        <v>-5</v>
+      </c>
+      <c r="C18" s="2">
+        <f>C$2*2^($B18/12)</f>
+        <v>329.62755691286992</v>
+      </c>
+      <c r="D18" s="11">
+        <f>$C18*D$1</f>
+        <v>659.25511382573984</v>
+      </c>
+      <c r="E18" s="2">
+        <f>$C18*E$1</f>
+        <v>988.8826707386097</v>
+      </c>
+      <c r="F18" s="7">
+        <f>$C18*F$1</f>
+        <v>1318.5102276514797</v>
+      </c>
+      <c r="G18" s="2">
+        <f>$C18*G$1</f>
+        <v>1648.1377845643497</v>
+      </c>
+      <c r="H18" s="2">
+        <f>$C18*H$1</f>
+        <v>1977.7653414772194</v>
+      </c>
+      <c r="I18" s="2">
+        <f>$C18*I$1</f>
+        <v>2307.3928983900896</v>
+      </c>
+      <c r="J18" s="2">
+        <f>$C18*J$1</f>
+        <v>2637.0204553029594</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19">
+        <v>-4</v>
+      </c>
+      <c r="C19" s="2">
+        <f>C$2*2^($B19/12)</f>
+        <v>349.22823143300388</v>
+      </c>
+      <c r="D19" s="2">
+        <f>$C19*D$1</f>
+        <v>698.45646286600777</v>
+      </c>
+      <c r="E19" s="2">
+        <f>$C19*E$1</f>
+        <v>1047.6846942990117</v>
+      </c>
+      <c r="F19" s="2">
+        <f>$C19*F$1</f>
+        <v>1396.9129257320155</v>
+      </c>
+      <c r="G19" s="6">
+        <f>$C19*G$1</f>
+        <v>1746.1411571650194</v>
+      </c>
+      <c r="H19" s="2">
+        <f>$C19*H$1</f>
+        <v>2095.3693885980233</v>
+      </c>
+      <c r="I19" s="2">
+        <f>$C19*I$1</f>
+        <v>2444.597620031027</v>
+      </c>
+      <c r="J19" s="2">
+        <f>$C19*J$1</f>
+        <v>2793.8258514640311</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20">
+        <v>-3</v>
+      </c>
+      <c r="C20" s="2">
+        <f>C$2*2^($B20/12)</f>
+        <v>369.99442271163446</v>
+      </c>
+      <c r="D20" s="2">
+        <f>$C20*D$1</f>
+        <v>739.98884542326891</v>
+      </c>
+      <c r="E20" s="10">
+        <f>$C20*E$1</f>
+        <v>1109.9832681349035</v>
+      </c>
+      <c r="F20" s="2">
+        <f>$C20*F$1</f>
+        <v>1479.9776908465378</v>
+      </c>
+      <c r="G20" s="2">
+        <f>$C20*G$1</f>
+        <v>1849.9721135581722</v>
+      </c>
+      <c r="H20" s="2">
+        <f>$C20*H$1</f>
+        <v>2219.966536269807</v>
+      </c>
+      <c r="I20" s="2">
+        <f>$C20*I$1</f>
+        <v>2589.9609589814413</v>
+      </c>
+      <c r="J20" s="2">
+        <f>$C20*J$1</f>
+        <v>2959.9553816930757</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="3">
+        <v>-2</v>
+      </c>
+      <c r="C21" s="2">
+        <f>C$2*2^($B21/12)</f>
+        <v>391.99543598174927</v>
+      </c>
+      <c r="D21" s="2">
+        <f>$C21*D$1</f>
+        <v>783.99087196349853</v>
+      </c>
+      <c r="E21" s="2">
+        <f>$C21*E$1</f>
+        <v>1175.9863079452477</v>
+      </c>
+      <c r="F21" s="9">
+        <f>$C21*F$1</f>
+        <v>1567.9817439269971</v>
+      </c>
+      <c r="G21" s="2">
+        <f>$C21*G$1</f>
+        <v>1959.9771799087464</v>
+      </c>
+      <c r="H21" s="2">
+        <f>$C21*H$1</f>
+        <v>2351.9726158904955</v>
+      </c>
+      <c r="I21" s="2">
+        <f>$C21*I$1</f>
+        <v>2743.9680518722448</v>
+      </c>
+      <c r="J21" s="2">
+        <f>$C21*J$1</f>
+        <v>3135.9634878539941</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22">
+        <v>-1</v>
+      </c>
+      <c r="C22" s="2">
+        <f>C$2*2^($B22/12)</f>
+        <v>415.30469757994513</v>
+      </c>
+      <c r="D22" s="2">
+        <f>$C22*D$1</f>
+        <v>830.60939515989025</v>
+      </c>
+      <c r="E22" s="2">
+        <f>$C22*E$1</f>
+        <v>1245.9140927398353</v>
+      </c>
+      <c r="F22" s="2">
+        <f>$C22*F$1</f>
+        <v>1661.2187903197805</v>
+      </c>
+      <c r="G22" s="2">
+        <f>$C22*G$1</f>
+        <v>2076.5234878997258</v>
+      </c>
+      <c r="H22" s="2">
+        <f>$C22*H$1</f>
+        <v>2491.8281854796705</v>
+      </c>
+      <c r="I22" s="2">
+        <f>$C22*I$1</f>
+        <v>2907.1328830596158</v>
+      </c>
+      <c r="J22" s="2">
+        <f>$C22*J$1</f>
+        <v>3322.437580639561</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="4">
+        <v>0</v>
+      </c>
+      <c r="C23" s="5">
+        <f>C$2*2^($B23/12)</f>
+        <v>440</v>
+      </c>
+      <c r="D23" s="8">
+        <f>$C23*D$1</f>
+        <v>880</v>
+      </c>
+      <c r="E23" s="7">
+        <f>$C23*E$1</f>
+        <v>1320</v>
+      </c>
+      <c r="F23" s="6">
+        <f>$C23*F$1</f>
+        <v>1760</v>
+      </c>
+      <c r="G23" s="5">
+        <f>$C23*G$1</f>
+        <v>2200</v>
+      </c>
+      <c r="H23" s="5">
+        <f>$C23*H$1</f>
+        <v>2640</v>
+      </c>
+      <c r="I23" s="5">
+        <f>$C23*I$1</f>
+        <v>3080</v>
+      </c>
+      <c r="J23" s="5">
+        <f>$C23*J$1</f>
+        <v>3520</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2">
+        <f>C$2*2^($B24/12)</f>
+        <v>466.16376151808993</v>
+      </c>
+      <c r="D24" s="2">
+        <f>$C24*D$1</f>
+        <v>932.32752303617985</v>
+      </c>
+      <c r="E24" s="2">
+        <f>$C24*E$1</f>
+        <v>1398.4912845542699</v>
+      </c>
+      <c r="F24" s="2">
+        <f>$C24*F$1</f>
+        <v>1864.6550460723597</v>
+      </c>
+      <c r="G24" s="2">
+        <f>$C24*G$1</f>
+        <v>2330.8188075904495</v>
+      </c>
+      <c r="H24" s="2">
+        <f>$C24*H$1</f>
+        <v>2796.9825691085398</v>
+      </c>
+      <c r="I24" s="2">
+        <f>$C24*I$1</f>
+        <v>3263.1463306266296</v>
+      </c>
+      <c r="J24" s="2">
+        <f>$C24*J$1</f>
+        <v>3729.3100921447194</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="3">
+        <v>2</v>
+      </c>
+      <c r="C25" s="2">
+        <f>C$2*2^($B25/12)</f>
+        <v>493.88330125612413</v>
+      </c>
+      <c r="D25" s="2">
+        <f>$C25*D$1</f>
+        <v>987.76660251224826</v>
+      </c>
+      <c r="E25" s="2">
+        <f>$C25*E$1</f>
+        <v>1481.6499037683725</v>
+      </c>
+      <c r="F25" s="2">
+        <f>$C25*F$1</f>
+        <v>1975.5332050244965</v>
+      </c>
+      <c r="G25" s="2">
+        <f>$C25*G$1</f>
+        <v>2469.4165062806205</v>
+      </c>
+      <c r="H25" s="2">
+        <f>$C25*H$1</f>
+        <v>2963.299807536745</v>
+      </c>
+      <c r="I25" s="2">
+        <f>$C25*I$1</f>
+        <v>3457.183108792869</v>
+      </c>
+      <c r="J25" s="2">
+        <f>$C25*J$1</f>
+        <v>3951.066410048993</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>1320</v>
+      </c>
+      <c r="C29" s="2">
+        <f>MIN(ABS(C11-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="D29" s="2">
+        <f>MIN(ABS(D11-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="E29" s="2">
+        <f>MIN(ABS(E11-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="F29" s="2">
+        <f>MIN(ABS(F11-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="G29" s="2">
+        <f>MIN(ABS(G11-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="H29" s="2">
+        <f>MIN(ABS(H11-$B$29),100)</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="2">
+        <f>MIN(ABS(I11-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="J29" s="2">
+        <f>MIN(ABS(J11-$B$29),100)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C30" s="2">
+        <f>MIN(ABS(C12-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="D30" s="2">
+        <f>MIN(ABS(D12-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="E30" s="2">
+        <f>MIN(ABS(E12-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="F30" s="2">
+        <f>MIN(ABS(F12-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="G30" s="2">
+        <f>MIN(ABS(G12-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="H30" s="2">
+        <f>MIN(ABS(H12-$B$29),100)</f>
+        <v>78.491284554269896</v>
+      </c>
+      <c r="I30" s="2">
+        <f>MIN(ABS(I12-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="J30" s="2">
+        <f>MIN(ABS(J12-$B$29),100)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C31" s="2">
+        <f>MIN(ABS(C13-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="D31" s="2">
+        <f>MIN(ABS(D13-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="E31" s="2">
+        <f>MIN(ABS(E13-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="F31" s="2">
+        <f>MIN(ABS(F13-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="G31" s="2">
+        <f>MIN(ABS(G13-$B$29),100)</f>
+        <v>85.291746859689738</v>
+      </c>
+      <c r="H31" s="2">
+        <f>MIN(ABS(H13-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="I31" s="2">
+        <f>MIN(ABS(I13-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="J31" s="2">
+        <f>MIN(ABS(J13-$B$29),100)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C32" s="2">
+        <f>MIN(ABS(C14-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="D32" s="2">
+        <f>MIN(ABS(D14-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="E32" s="2">
+        <f>MIN(ABS(E14-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="F32" s="2">
+        <f>MIN(ABS(F14-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="G32" s="2">
+        <f>MIN(ABS(G14-$B$29),100)</f>
+        <v>11.87217349700677</v>
+      </c>
+      <c r="H32" s="2">
+        <f>MIN(ABS(H14-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="I32" s="2">
+        <f>MIN(ABS(I14-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="J32" s="2">
+        <f>MIN(ABS(J14-$B$29),100)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C33" s="2">
+        <f>MIN(ABS(C15-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="D33" s="2">
+        <f>MIN(ABS(D15-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="E33" s="2">
+        <f>MIN(ABS(E15-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="F33" s="2">
+        <f>MIN(ABS(F15-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="G33" s="2">
+        <f>MIN(ABS(G15-$B$29),100)</f>
+        <v>65.913154884360438</v>
+      </c>
+      <c r="H33" s="2">
+        <f>MIN(ABS(H15-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="I33" s="2">
+        <f>MIN(ABS(I15-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="J33" s="2">
+        <f>MIN(ABS(J15-$B$29),100)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C34" s="2">
+        <f>MIN(ABS(C16-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="D34" s="2">
+        <f>MIN(ABS(D16-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="E34" s="2">
+        <f>MIN(ABS(E16-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="F34" s="2">
+        <f>MIN(ABS(F16-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="G34" s="2">
+        <f>MIN(ABS(G16-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="H34" s="2">
+        <f>MIN(ABS(H16-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="I34" s="2">
+        <f>MIN(ABS(I16-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="J34" s="2">
+        <f>MIN(ABS(J16-$B$29),100)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C35" s="2">
+        <f>MIN(ABS(C17-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="D35" s="2">
+        <f>MIN(ABS(D17-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="E35" s="2">
+        <f>MIN(ABS(E17-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="F35" s="2">
+        <f>MIN(ABS(F17-$B$29),100)</f>
+        <v>75.492065111676538</v>
+      </c>
+      <c r="G35" s="2">
+        <f>MIN(ABS(G17-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="H35" s="2">
+        <f>MIN(ABS(H17-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="I35" s="2">
+        <f>MIN(ABS(I17-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="J35" s="2">
+        <f>MIN(ABS(J17-$B$29),100)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C36" s="2">
+        <f>MIN(ABS(C18-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="D36" s="2">
+        <f>MIN(ABS(D18-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="E36" s="2">
+        <f>MIN(ABS(E18-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="F36" s="2">
+        <f>MIN(ABS(F18-$B$29),100)</f>
+        <v>1.4897723485203187</v>
+      </c>
+      <c r="G36" s="2">
+        <f>MIN(ABS(G18-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="H36" s="2">
+        <f>MIN(ABS(H18-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="I36" s="2">
+        <f>MIN(ABS(I18-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="J36" s="2">
+        <f>MIN(ABS(J18-$B$29),100)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C37" s="2">
+        <f>MIN(ABS(C19-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="D37" s="2">
+        <f>MIN(ABS(D19-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="E37" s="2">
+        <f>MIN(ABS(E19-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="F37" s="2">
+        <f>MIN(ABS(F19-$B$29),100)</f>
+        <v>76.912925732015538</v>
+      </c>
+      <c r="G37" s="2">
+        <f>MIN(ABS(G19-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="H37" s="2">
+        <f>MIN(ABS(H19-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="I37" s="2">
+        <f>MIN(ABS(I19-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="J37" s="2">
+        <f>MIN(ABS(J19-$B$29),100)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C38" s="2">
+        <f>MIN(ABS(C20-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="D38" s="2">
+        <f>MIN(ABS(D20-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="E38" s="2">
+        <f>MIN(ABS(E20-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="F38" s="2">
+        <f>MIN(ABS(F20-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="G38" s="2">
+        <f>MIN(ABS(G20-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="H38" s="2">
+        <f>MIN(ABS(H20-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="I38" s="2">
+        <f>MIN(ABS(I20-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="J38" s="2">
+        <f>MIN(ABS(J20-$B$29),100)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C39" s="2">
+        <f>MIN(ABS(C21-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="D39" s="2">
+        <f>MIN(ABS(D21-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="E39" s="2">
+        <f>MIN(ABS(E21-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="F39" s="2">
+        <f>MIN(ABS(F21-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="G39" s="2">
+        <f>MIN(ABS(G21-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="H39" s="2">
+        <f>MIN(ABS(H21-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="I39" s="2">
+        <f>MIN(ABS(I21-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="J39" s="2">
+        <f>MIN(ABS(J21-$B$29),100)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C40" s="2">
+        <f>MIN(ABS(C22-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="D40" s="2">
+        <f>MIN(ABS(D22-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="E40" s="2">
+        <f>MIN(ABS(E22-$B$29),100)</f>
+        <v>74.085907260164731</v>
+      </c>
+      <c r="F40" s="2">
+        <f>MIN(ABS(F22-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="G40" s="2">
+        <f>MIN(ABS(G22-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="H40" s="2">
+        <f>MIN(ABS(H22-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="I40" s="2">
+        <f>MIN(ABS(I22-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="J40" s="2">
+        <f>MIN(ABS(J22-$B$29),100)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C41" s="2">
+        <f>MIN(ABS(C23-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="D41" s="2">
+        <f>MIN(ABS(D23-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="E41" s="2">
+        <f>MIN(ABS(E23-$B$29),100)</f>
+        <v>0</v>
+      </c>
+      <c r="F41" s="2">
+        <f>MIN(ABS(F23-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="G41" s="2">
+        <f>MIN(ABS(G23-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="H41" s="2">
+        <f>MIN(ABS(H23-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="I41" s="2">
+        <f>MIN(ABS(I23-$B$29),100)</f>
+        <v>100</v>
+      </c>
+      <c r="J41" s="2">
+        <f>MIN(ABS(J23-$B$29),100)</f>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C29:J41">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddHeader>&amp;R&amp;"Calibri"&amp;12&amp;KFF8C00 CONFIDENTIAL &amp; RESTRICTED&amp;1#_x000D_</oddHeader>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C05824F7-8E91-B44E-B48B-0568FF81ED85}">
   <dimension ref="A1:J89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
@@ -4227,7 +5723,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{290CCE15-D2E0-BD4B-BA4B-DB7A9F159085}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -4239,163 +5735,163 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
-        <f>Harmonique!B34</f>
+        <f>Harmoniques!B34</f>
         <v>FA3</v>
       </c>
       <c r="B1" t="str">
-        <f>Harmonique!B38</f>
+        <f>Harmoniques!B38</f>
         <v>LA3</v>
       </c>
       <c r="C1">
-        <f>Harmonique!G34</f>
+        <f>Harmoniques!G34</f>
         <v>873.07057858250982</v>
       </c>
       <c r="D1">
-        <f>Harmonique!F38</f>
+        <f>Harmoniques!F38</f>
         <v>880</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
-        <f>Harmonique!B35</f>
+        <f>Harmoniques!B35</f>
         <v>FA#3</v>
       </c>
       <c r="B2" t="str">
-        <f>Harmonique!B39</f>
+        <f>Harmoniques!B39</f>
         <v>LA#3</v>
       </c>
       <c r="C2">
-        <f>Harmonique!G35</f>
+        <f>Harmoniques!G35</f>
         <v>924.98605677908608</v>
       </c>
       <c r="D2">
-        <f>Harmonique!F39</f>
+        <f>Harmoniques!F39</f>
         <v>932.32752303617985</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
-        <f>Harmonique!B36</f>
+        <f>Harmoniques!B36</f>
         <v>SOL</v>
       </c>
       <c r="B3" t="str">
-        <f>Harmonique!B40</f>
+        <f>Harmoniques!B40</f>
         <v>SI3</v>
       </c>
       <c r="C3">
-        <f>Harmonique!G36</f>
+        <f>Harmoniques!G36</f>
         <v>979.9885899543732</v>
       </c>
       <c r="D3">
-        <f>Harmonique!F40</f>
+        <f>Harmoniques!F40</f>
         <v>987.76660251224826</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
-        <f>Harmonique!B37</f>
+        <f>Harmoniques!B37</f>
         <v>SOL#3</v>
       </c>
       <c r="B4" t="str">
-        <f>Harmonique!B41</f>
+        <f>Harmoniques!B41</f>
         <v>DO4</v>
       </c>
       <c r="C4">
-        <f>Harmonique!G37</f>
+        <f>Harmoniques!G37</f>
         <v>1038.2617439498629</v>
       </c>
       <c r="D4">
-        <f>Harmonique!F41</f>
+        <f>Harmoniques!F41</f>
         <v>1046.5022612023945</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
-        <f>Harmonique!B38</f>
+        <f>Harmoniques!B38</f>
         <v>LA3</v>
       </c>
       <c r="B5" t="str">
-        <f>Harmonique!B42</f>
+        <f>Harmoniques!B42</f>
         <v>DO#4</v>
       </c>
       <c r="C5">
-        <f>Harmonique!G38</f>
+        <f>Harmoniques!G38</f>
         <v>1100</v>
       </c>
       <c r="D5">
-        <f>Harmonique!F42</f>
+        <f>Harmoniques!F42</f>
         <v>1108.7305239074883</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
-        <f>Harmonique!B39</f>
+        <f>Harmoniques!B39</f>
         <v>LA#3</v>
       </c>
       <c r="B6" t="str">
-        <f>Harmonique!B43</f>
+        <f>Harmoniques!B43</f>
         <v>RE4</v>
       </c>
       <c r="C6">
-        <f>Harmonique!G39</f>
+        <f>Harmoniques!G39</f>
         <v>1165.4094037952248</v>
       </c>
       <c r="D6">
-        <f>Harmonique!F43</f>
+        <f>Harmoniques!F43</f>
         <v>1174.6590716696303</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
-        <f>Harmonique!B40</f>
+        <f>Harmoniques!B40</f>
         <v>SI3</v>
       </c>
       <c r="B7" t="str">
-        <f>Harmonique!B44</f>
+        <f>Harmoniques!B44</f>
         <v>RE#4</v>
       </c>
       <c r="C7">
-        <f>Harmonique!G40</f>
+        <f>Harmoniques!G40</f>
         <v>1234.7082531403103</v>
       </c>
       <c r="D7">
-        <f>Harmonique!F44</f>
+        <f>Harmoniques!F44</f>
         <v>1244.5079348883235</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
-        <f>Harmonique!B41</f>
+        <f>Harmoniques!B41</f>
         <v>DO4</v>
       </c>
       <c r="B8" t="str">
-        <f>Harmonique!B45</f>
+        <f>Harmoniques!B45</f>
         <v>MI4</v>
       </c>
       <c r="C8">
-        <f>Harmonique!G41</f>
+        <f>Harmoniques!G41</f>
         <v>1308.1278265029932</v>
       </c>
       <c r="D8">
-        <f>Harmonique!F45</f>
+        <f>Harmoniques!F45</f>
         <v>1318.5102276514797</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
-        <f>Harmonique!B42</f>
+        <f>Harmoniques!B42</f>
         <v>DO#4</v>
       </c>
       <c r="B9" t="str">
-        <f>Harmonique!B46</f>
+        <f>Harmoniques!B46</f>
         <v>FA4</v>
       </c>
       <c r="C9">
-        <f>Harmonique!G42</f>
+        <f>Harmoniques!G42</f>
         <v>1385.9131548843604</v>
       </c>
       <c r="D9">
-        <f>Harmonique!F46</f>
+        <f>Harmoniques!F46</f>
         <v>1396.9129257320155</v>
       </c>
     </row>
@@ -4404,7 +5900,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF9A8EF6-406B-EE46-8AFC-D0151277055B}">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -4416,145 +5912,145 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="str">
-        <f>Harmonique!B34</f>
+        <f>Harmoniques!B34</f>
         <v>FA3</v>
       </c>
       <c r="B1" s="1" t="str">
-        <f>Harmonique!B39</f>
+        <f>Harmoniques!B39</f>
         <v>LA#3</v>
       </c>
       <c r="C1" s="1">
-        <f>Harmonique!F34</f>
+        <f>Harmoniques!F34</f>
         <v>698.45646286600788</v>
       </c>
       <c r="D1" s="1">
-        <f>Harmonique!E39</f>
+        <f>Harmoniques!E39</f>
         <v>699.24564227713495</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="str">
-        <f>Harmonique!B35</f>
+        <f>Harmoniques!B35</f>
         <v>FA#3</v>
       </c>
       <c r="B2" s="1" t="str">
-        <f>Harmonique!B40</f>
+        <f>Harmoniques!B40</f>
         <v>SI3</v>
       </c>
       <c r="C2" s="1">
-        <f>Harmonique!F35</f>
+        <f>Harmoniques!F35</f>
         <v>739.98884542326891</v>
       </c>
       <c r="D2" s="1">
-        <f>Harmonique!E40</f>
+        <f>Harmoniques!E40</f>
         <v>740.82495188418625</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="str">
-        <f>Harmonique!B36</f>
+        <f>Harmoniques!B36</f>
         <v>SOL</v>
       </c>
       <c r="B3" s="1" t="str">
-        <f>Harmonique!B41</f>
+        <f>Harmoniques!B41</f>
         <v>DO4</v>
       </c>
       <c r="C3" s="1">
-        <f>Harmonique!F36</f>
+        <f>Harmoniques!F36</f>
         <v>783.99087196349853</v>
       </c>
       <c r="D3" s="1">
-        <f>Harmonique!E41</f>
+        <f>Harmoniques!E41</f>
         <v>784.87669590179587</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="str">
-        <f>Harmonique!B37</f>
+        <f>Harmoniques!B37</f>
         <v>SOL#3</v>
       </c>
       <c r="B4" s="1" t="str">
-        <f>Harmonique!B42</f>
+        <f>Harmoniques!B42</f>
         <v>DO#4</v>
       </c>
       <c r="C4" s="1">
-        <f>Harmonique!F37</f>
+        <f>Harmoniques!F37</f>
         <v>830.60939515989037</v>
       </c>
       <c r="D4" s="1">
-        <f>Harmonique!E42</f>
+        <f>Harmoniques!E42</f>
         <v>831.54789293061617</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="str">
-        <f>Harmonique!B38</f>
+        <f>Harmoniques!B38</f>
         <v>LA3</v>
       </c>
       <c r="B5" s="1" t="str">
-        <f>Harmonique!B43</f>
+        <f>Harmoniques!B43</f>
         <v>RE4</v>
       </c>
       <c r="C5" s="1">
-        <f>Harmonique!F38</f>
+        <f>Harmoniques!F38</f>
         <v>880</v>
       </c>
       <c r="D5" s="1">
-        <f>Harmonique!E43</f>
+        <f>Harmoniques!E43</f>
         <v>880.99430375222278</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="str">
-        <f>Harmonique!B39</f>
+        <f>Harmoniques!B39</f>
         <v>LA#3</v>
       </c>
       <c r="B6" s="1" t="str">
-        <f>Harmonique!B44</f>
+        <f>Harmoniques!B44</f>
         <v>RE#4</v>
       </c>
       <c r="C6" s="1">
-        <f>Harmonique!F39</f>
+        <f>Harmoniques!F39</f>
         <v>932.32752303617985</v>
       </c>
       <c r="D6" s="1">
-        <f>Harmonique!E44</f>
+        <f>Harmoniques!E44</f>
         <v>933.38095116624254</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="str">
-        <f>Harmonique!B40</f>
+        <f>Harmoniques!B40</f>
         <v>SI3</v>
       </c>
       <c r="B7" s="1" t="str">
-        <f>Harmonique!B45</f>
+        <f>Harmoniques!B45</f>
         <v>MI4</v>
       </c>
       <c r="C7" s="1">
-        <f>Harmonique!F40</f>
+        <f>Harmoniques!F40</f>
         <v>987.76660251224826</v>
       </c>
       <c r="D7" s="1">
-        <f>Harmonique!E45</f>
+        <f>Harmoniques!E45</f>
         <v>988.8826707386097</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="str">
-        <f>Harmonique!B41</f>
+        <f>Harmoniques!B41</f>
         <v>DO4</v>
       </c>
       <c r="B8" s="1" t="str">
-        <f>Harmonique!B46</f>
+        <f>Harmoniques!B46</f>
         <v>FA4</v>
       </c>
       <c r="C8" s="1">
-        <f>Harmonique!F41</f>
+        <f>Harmoniques!F41</f>
         <v>1046.5022612023945</v>
       </c>
       <c r="D8" s="1">
-        <f>Harmonique!E46</f>
+        <f>Harmoniques!E46</f>
         <v>1047.6846942990117</v>
       </c>
     </row>
@@ -4563,7 +6059,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9832D34-03D3-CD45-9734-E855E685ADC2}">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -4575,109 +6071,109 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
-        <f>Harmonique!B34</f>
+        <f>Harmoniques!B34</f>
         <v>FA3</v>
       </c>
       <c r="B1" t="str">
-        <f>Harmonique!B41</f>
+        <f>Harmoniques!B41</f>
         <v>DO4</v>
       </c>
       <c r="C1">
-        <f>Harmonique!E34</f>
+        <f>Harmoniques!E34</f>
         <v>523.84234714950594</v>
       </c>
       <c r="D1">
-        <f>Harmonique!D41</f>
+        <f>Harmoniques!D41</f>
         <v>523.25113060119725</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
-        <f>Harmonique!B35</f>
+        <f>Harmoniques!B35</f>
         <v>FA#3</v>
       </c>
       <c r="B2" t="str">
-        <f>Harmonique!B42</f>
+        <f>Harmoniques!B42</f>
         <v>DO#4</v>
       </c>
       <c r="C2">
-        <f>Harmonique!E35</f>
+        <f>Harmoniques!E35</f>
         <v>554.99163406745174</v>
       </c>
       <c r="D2">
-        <f>Harmonique!D42</f>
+        <f>Harmoniques!D42</f>
         <v>554.36526195374415</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
-        <f>Harmonique!B36</f>
+        <f>Harmoniques!B36</f>
         <v>SOL</v>
       </c>
       <c r="B3" t="str">
-        <f>Harmonique!B43</f>
+        <f>Harmoniques!B43</f>
         <v>RE4</v>
       </c>
       <c r="C3">
-        <f>Harmonique!E36</f>
+        <f>Harmoniques!E36</f>
         <v>587.99315397262387</v>
       </c>
       <c r="D3">
-        <f>Harmonique!D43</f>
+        <f>Harmoniques!D43</f>
         <v>587.32953583481515</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
-        <f>Harmonique!B37</f>
+        <f>Harmoniques!B37</f>
         <v>SOL#3</v>
       </c>
       <c r="B4" t="str">
-        <f>Harmonique!B44</f>
+        <f>Harmoniques!B44</f>
         <v>RE#4</v>
       </c>
       <c r="C4">
-        <f>Harmonique!E37</f>
+        <f>Harmoniques!E37</f>
         <v>622.95704636991775</v>
       </c>
       <c r="D4">
-        <f>Harmonique!D44</f>
+        <f>Harmoniques!D44</f>
         <v>622.25396744416173</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
-        <f>Harmonique!B38</f>
+        <f>Harmoniques!B38</f>
         <v>LA3</v>
       </c>
       <c r="B5" t="str">
-        <f>Harmonique!B45</f>
+        <f>Harmoniques!B45</f>
         <v>MI4</v>
       </c>
       <c r="C5">
-        <f>Harmonique!E38</f>
+        <f>Harmoniques!E38</f>
         <v>660</v>
       </c>
       <c r="D5">
-        <f>Harmonique!D45</f>
+        <f>Harmoniques!D45</f>
         <v>659.25511382573984</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
-        <f>Harmonique!B39</f>
+        <f>Harmoniques!B39</f>
         <v>LA#3</v>
       </c>
       <c r="B6" t="str">
-        <f>Harmonique!B46</f>
+        <f>Harmoniques!B46</f>
         <v>FA4</v>
       </c>
       <c r="C6">
-        <f>Harmonique!E39</f>
+        <f>Harmoniques!E39</f>
         <v>699.24564227713495</v>
       </c>
       <c r="D6">
-        <f>Harmonique!D46</f>
+        <f>Harmoniques!D46</f>
         <v>698.45646286600777</v>
       </c>
     </row>
@@ -4686,7 +6182,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5347174-07C9-F14F-B918-0473F22E553D}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -4698,73 +6194,73 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
-        <f>Harmonique!B34</f>
+        <f>Harmoniques!B34</f>
         <v>FA3</v>
       </c>
       <c r="B1" t="str">
-        <f>Harmonique!B43</f>
+        <f>Harmoniques!B43</f>
         <v>RE4</v>
       </c>
       <c r="C1">
-        <f>Harmonique!G34</f>
+        <f>Harmoniques!G34</f>
         <v>873.07057858250982</v>
       </c>
       <c r="D1">
-        <f>Harmonique!E43</f>
+        <f>Harmoniques!E43</f>
         <v>880.99430375222278</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
-        <f>Harmonique!B35</f>
+        <f>Harmoniques!B35</f>
         <v>FA#3</v>
       </c>
       <c r="B2" t="str">
-        <f>Harmonique!B44</f>
+        <f>Harmoniques!B44</f>
         <v>RE#4</v>
       </c>
       <c r="C2">
-        <f>Harmonique!G35</f>
+        <f>Harmoniques!G35</f>
         <v>924.98605677908608</v>
       </c>
       <c r="D2">
-        <f>Harmonique!E44</f>
+        <f>Harmoniques!E44</f>
         <v>933.38095116624254</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
-        <f>Harmonique!B36</f>
+        <f>Harmoniques!B36</f>
         <v>SOL</v>
       </c>
       <c r="B3" t="str">
-        <f>Harmonique!B45</f>
+        <f>Harmoniques!B45</f>
         <v>MI4</v>
       </c>
       <c r="C3">
-        <f>Harmonique!G36</f>
+        <f>Harmoniques!G36</f>
         <v>979.9885899543732</v>
       </c>
       <c r="D3">
-        <f>Harmonique!E45</f>
+        <f>Harmoniques!E45</f>
         <v>988.8826707386097</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
-        <f>Harmonique!B37</f>
+        <f>Harmoniques!B37</f>
         <v>SOL#3</v>
       </c>
       <c r="B4" t="str">
-        <f>Harmonique!B46</f>
+        <f>Harmoniques!B46</f>
         <v>FA4</v>
       </c>
       <c r="C4">
-        <f>Harmonique!G37</f>
+        <f>Harmoniques!G37</f>
         <v>1038.2617439498629</v>
       </c>
       <c r="D4">
-        <f>Harmonique!E46</f>
+        <f>Harmoniques!E46</f>
         <v>1047.6846942990117</v>
       </c>
     </row>

</xml_diff>